<commit_message>
worked on arithmetic operations and refactored authentication
</commit_message>
<xml_diff>
--- a/src/databases/test-data/users_db.xlsx
+++ b/src/databases/test-data/users_db.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coded\OneDrive\Desktop\loanpro-challenge-aws-lambda-backend\src\databases\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADEC552-3E19-4EAE-9C5E-32136CFBEB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F020DC4-463E-496D-B112-DF39146FB12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="1185" windowWidth="18915" windowHeight="11295" xr2:uid="{6D1F38E0-FFAB-4BB8-A9B4-F06A05BAE4DD}"/>
+    <workbookView xWindow="18420" yWindow="2475" windowWidth="18915" windowHeight="11295" activeTab="1" xr2:uid="{6D1F38E0-FFAB-4BB8-A9B4-F06A05BAE4DD}"/>
   </bookViews>
   <sheets>
     <sheet name="UsersTable" sheetId="1" r:id="rId1"/>
+    <sheet name="UsersBalances" sheetId="2" r:id="rId2"/>
+    <sheet name="UsersOperationsRecords" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>7902a95978eac488ee86b560c2d9f17e82d3c66a86068c30fe488cc8e4edea0e</t>
   </si>
@@ -63,6 +65,18 @@
   </si>
   <si>
     <t>inactive</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>balance</t>
+  </si>
+  <si>
+    <t>records</t>
+  </si>
+  <si>
+    <t>{}</t>
   </si>
 </sst>
 </file>
@@ -107,10 +121,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -428,7 +444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2096B643-3AEC-405E-9E59-474499644869}">
   <dimension ref="A1:D1961"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -6361,4 +6377,93 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A46205F7-6A7E-4259-BB8C-187AA93A2283}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>100000.53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A710645-ACEE-4922-B39A-192F8C4B95D6}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>